<commit_message>
Updated the configfrile and the initial workflow's selector for activities that needs UI interaction
</commit_message>
<xml_diff>
--- a/WAHPConfigFile.xlsx
+++ b/WAHPConfigFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\WAHPMatchingAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{438B3EA4-8E48-478A-B3C5-A4CEB95C4D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04F8CCC-597A-4BBB-A852-72D1045A71C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12690" yWindow="-630" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
@@ -159,9 +159,6 @@
     <t>lester.rollan@lexisnexisrisk.com</t>
   </si>
   <si>
-    <t>https://reedelsevier.sharepoint.com/sites/OG-CRUOps-RARIncoming/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DCRUOps%2DRARIncoming%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DCRUOps%2DRARIncoming%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DCRUOps%2DRARIncoming%2FShared%20Documents%2FWA%5FHP%2F</t>
-  </si>
-  <si>
     <t>%2FDONE&amp;viewid=8a644220%2Dba9b%2D4af3%2Db3bb%2De9cda30e1eae</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Desktop\WAHP</t>
+  </si>
+  <si>
+    <t>https://reedelsevier.sharepoint.com/sites/OG-CRUOps-RARIncoming/Shared%20Documents/Forms/AllItems.aspx?id=%2Fsites%2FOG%2DCRUOps%2DRARIncoming%2FShared%20Documents%2FWA%5FHP%2FWABOT%2F</t>
   </si>
 </sst>
 </file>
@@ -266,10 +266,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -607,14 +607,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FCB039-29A7-49D1-BD2D-CAC9DFC1D441}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="77.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="84.85546875" style="2" customWidth="1"/>
     <col min="3" max="3" width="45.140625" style="2" customWidth="1"/>
     <col min="4" max="16384" width="32.85546875" style="2"/>
   </cols>
@@ -641,37 +641,37 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>41</v>
+      <c r="B4" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>41</v>
+      <c r="B5" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -679,7 +679,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
@@ -700,8 +700,8 @@
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>46</v>
+      <c r="B8" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>23</v>
@@ -777,7 +777,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://reedelsevier.sharepoint.com/sites/OG-CRUOps-RARIncoming/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DCRUOps%2DRARIncoming%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DCRUOps%2DRARIncoming%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DCRUOps%2DRARIncoming%2FShared%20Documents%2FWA%5FHP%2F" xr:uid="{AE603AE5-8317-43DD-94B6-FAA4A34FF1BA}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{AE603AE5-8317-43DD-94B6-FAA4A34FF1BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -799,11 +799,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -937,11 +937,11 @@
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1065,11 +1065,11 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="A29" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">

</xml_diff>

<commit_message>
Updates done: - Flow updated for the donwloaded files to be saved in the default "Downloads" folder - Flow updated to move the downloaded files from the "Dwonloads" folder to the MasterFolder
</commit_message>
<xml_diff>
--- a/WAHPConfigFile.xlsx
+++ b/WAHPConfigFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\WAHPMatchingAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04F8CCC-597A-4BBB-A852-72D1045A71C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80485104-1D9C-499F-BC57-B027ADD56627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12690" yWindow="-630" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -156,28 +156,37 @@
     <t>lester.rollan@lexisnexisrisk.com; dindee.galindo@lexisnexisrisk.com; jesriel.tolentino@lexisnexisrisk.com; jhoanna.talle@lexisnexisrisk.com; paul.fabro@lexisnexisrisk.com; judy.cotaoco@lexisnexisrisk.com</t>
   </si>
   <si>
+    <t>%2FDONE&amp;viewid=8a644220%2Dba9b%2D4af3%2Db3bb%2De9cda30e1eae</t>
+  </si>
+  <si>
+    <t>SharePoint site's WAHP folder - base URL</t>
+  </si>
+  <si>
+    <t>SharePoint site's WAHP DONE folder</t>
+  </si>
+  <si>
+    <t>SharePoint site's WAHP folder - suffix URL (after current date)</t>
+  </si>
+  <si>
+    <t>C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Desktop\WAHP\</t>
+  </si>
+  <si>
+    <t>C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Desktop\WAHP</t>
+  </si>
+  <si>
+    <t>https://reedelsevier.sharepoint.com/sites/OG-CRUOps-RARIncoming/Shared%20Documents/Forms/AllItems.aspx?id=%2Fsites%2FOG%2DCRUOps%2DRARIncoming%2FShared%20Documents%2FWA%5FHP%2FWABOT%2F</t>
+  </si>
+  <si>
+    <t>DownloadsFolder</t>
+  </si>
+  <si>
+    <t>Download folder's path</t>
+  </si>
+  <si>
+    <t>C:\Users\RollLe01\Downloads\</t>
+  </si>
+  <si>
     <t>lester.rollan@lexisnexisrisk.com</t>
-  </si>
-  <si>
-    <t>%2FDONE&amp;viewid=8a644220%2Dba9b%2D4af3%2Db3bb%2De9cda30e1eae</t>
-  </si>
-  <si>
-    <t>SharePoint site's WAHP folder - base URL</t>
-  </si>
-  <si>
-    <t>SharePoint site's WAHP DONE folder</t>
-  </si>
-  <si>
-    <t>SharePoint site's WAHP folder - suffix URL (after current date)</t>
-  </si>
-  <si>
-    <t>C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Desktop\WAHP\</t>
-  </si>
-  <si>
-    <t>C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Desktop\WAHP</t>
-  </si>
-  <si>
-    <t>https://reedelsevier.sharepoint.com/sites/OG-CRUOps-RARIncoming/Shared%20Documents/Forms/AllItems.aspx?id=%2Fsites%2FOG%2DCRUOps%2DRARIncoming%2FShared%20Documents%2FWA%5FHP%2FWABOT%2F</t>
   </si>
 </sst>
 </file>
@@ -608,7 +617,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:C17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,10 +655,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -657,10 +666,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -668,10 +677,10 @@
         <v>8</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -679,7 +688,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
@@ -701,7 +710,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>23</v>
@@ -722,8 +731,8 @@
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>39</v>
+      <c r="B10" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
@@ -733,17 +742,23 @@
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>39</v>
+      <c r="B11" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
@@ -778,6 +793,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{AE603AE5-8317-43DD-94B6-FAA4A34FF1BA}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{30720489-4D4F-41E1-9615-2A1EB4ACD506}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{C6205818-EE13-4877-8FF0-69E4D8C05543}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
push after updating the packages
</commit_message>
<xml_diff>
--- a/WAHPConfigFile.xlsx
+++ b/WAHPConfigFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\WAHPMatchingAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80485104-1D9C-499F-BC57-B027ADD56627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD16BEF7-7CD9-41DD-9E1B-0E934212E4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -150,12 +150,6 @@
     <t>E:\Bot_Files\RPA FL Renaming\FLOBOT</t>
   </si>
   <si>
-    <t>sam.tecson@lexisnexisrisk.com; joavic.quisano@lexisnexisrisk.com; david.villasoto@lexisnexisrisk.com</t>
-  </si>
-  <si>
-    <t>lester.rollan@lexisnexisrisk.com; dindee.galindo@lexisnexisrisk.com; jesriel.tolentino@lexisnexisrisk.com; jhoanna.talle@lexisnexisrisk.com; paul.fabro@lexisnexisrisk.com; judy.cotaoco@lexisnexisrisk.com</t>
-  </si>
-  <si>
     <t>%2FDONE&amp;viewid=8a644220%2Dba9b%2D4af3%2Db3bb%2De9cda30e1eae</t>
   </si>
   <si>
@@ -186,7 +180,13 @@
     <t>C:\Users\RollLe01\Downloads\</t>
   </si>
   <si>
-    <t>lester.rollan@lexisnexisrisk.com</t>
+    <t>C:\Users\svc-RCOUIPBOT0005\Downloads\</t>
+  </si>
+  <si>
+    <t>jhoanna.talle@lexisnexisrisk.com; doris.cuaresma@lexisnexisrisk.com</t>
+  </si>
+  <si>
+    <t>agnes.sara@lexisnexisrisk.com; jomar.espos@lexisnexisrisk.com; gerard.mancenido@lexisnexisrisk.com; lester.rollan@lexisnexisrisk.com; dindee.galindo@lexisnexisrisk.com; jesriel.tolentino@lexisnexisrisk.com; paul.fabro@lexisnexisrisk.com; judy.cotaoco@lexisnexisrisk.com</t>
   </si>
 </sst>
 </file>
@@ -617,18 +617,18 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="32.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="84.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="32.85546875" style="2"/>
+    <col min="1" max="1" width="20.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="84.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.1796875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="32.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -639,7 +639,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -650,51 +650,51 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -705,18 +705,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -727,65 +727,65 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>49</v>
+      <c r="B10" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="1" t="s">
         <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -793,8 +793,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{AE603AE5-8317-43DD-94B6-FAA4A34FF1BA}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{30720489-4D4F-41E1-9615-2A1EB4ACD506}"/>
-    <hyperlink ref="B10" r:id="rId3" xr:uid="{C6205818-EE13-4877-8FF0-69E4D8C05543}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -802,27 +800,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:B23"/>
+    <sheetView topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="78.85546875" customWidth="1"/>
-    <col min="3" max="3" width="64.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="78.81640625" customWidth="1"/>
+    <col min="3" max="3" width="64.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -833,7 +831,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -844,7 +842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -855,7 +853,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -866,7 +864,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -877,7 +875,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -888,7 +886,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -899,7 +897,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -910,7 +908,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -921,46 +919,52 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
@@ -971,7 +975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -982,7 +986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -993,7 +997,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -1004,7 +1008,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -1015,7 +1019,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1026,7 +1030,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -1037,7 +1041,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1048,7 +1052,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1059,36 +1063,47 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1114,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -1110,7 +1125,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -1121,7 +1136,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -1132,7 +1147,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
@@ -1143,7 +1158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
@@ -1154,7 +1169,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
@@ -1165,7 +1180,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -1176,7 +1191,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
@@ -1187,26 +1202,37 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the following: - project package (UiPath.System.Activities) - Auto-email flow - ConfigFile
</commit_message>
<xml_diff>
--- a/WAHPConfigFile.xlsx
+++ b/WAHPConfigFile.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\WAHPMatchingAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Desktop\UiPath Projects\WAHPMatchingAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3165A7E8-66C0-4A8E-B096-C03E72048723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7717CA4B-87DC-488D-9C35-004D6AF64F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
@@ -198,7 +198,7 @@
     <t>agnes.sara@lexisnexisrisk.com; gerard.mancenido@lexisnexisrisk.com; lester.rollan@lexisnexisrisk.com; dindee.galindo@lexisnexisrisk.com; jesriel.tolentino@lexisnexisrisk.com; paul.fabro@lexisnexisrisk.com; judy.cotaoco@lexisnexisrisk.com</t>
   </si>
   <si>
-    <t>jhoanna.talle@lexisnexisrisk.com; doris.cuaresma@lexisnexisrisk.com; shiela.agravante@lexisnexisrisk.com</t>
+    <t>doris.cuaresma@lexisnexisrisk.com; shiela.agravante@lexisnexisrisk.com</t>
   </si>
 </sst>
 </file>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FCB039-29A7-49D1-BD2D-CAC9DFC1D441}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -739,7 +739,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -799,7 +799,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
+      <c r="B18" s="5"/>
       <c r="C18" s="1"/>
     </row>
   </sheetData>
@@ -812,10 +812,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:B20"/>
+    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45:B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1247,6 +1247,14 @@
       <c r="C41" s="1" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Updated package version for UiPath.UIAutomation.Activities Updated ConfigFile for package uploading in Orchestrator
</commit_message>
<xml_diff>
--- a/WAHPConfigFile.xlsx
+++ b/WAHPConfigFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Desktop\UiPath Projects\WAHPMatchingAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7717CA4B-87DC-488D-9C35-004D6AF64F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D26233-92AE-4905-BD30-EE85DB539E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -174,16 +174,7 @@
     <t>C:\Users\svc-RCOUIPBOT0005\Downloads\</t>
   </si>
   <si>
-    <t>jhoanna.talle@lexisnexisrisk.com; doris.cuaresma@lexisnexisrisk.com</t>
-  </si>
-  <si>
-    <t>agnes.sara@lexisnexisrisk.com; jomar.espos@lexisnexisrisk.com; gerard.mancenido@lexisnexisrisk.com; lester.rollan@lexisnexisrisk.com; dindee.galindo@lexisnexisrisk.com; jesriel.tolentino@lexisnexisrisk.com; paul.fabro@lexisnexisrisk.com; judy.cotaoco@lexisnexisrisk.com</t>
-  </si>
-  <si>
     <t>https://reedelsevier.sharepoint.com/sites/RollanLester/Shared%20Documents/Forms/AllItems.aspx?id=%2Fsites%2FRollanLester%2FShared%20Documents%2FWAHP&amp;viewid=105abaaa%2D085a%2D4a79%2D8458%2D7b6ecbd5487b</t>
-  </si>
-  <si>
-    <t>lester.rollan@lexisnexisrisk.com</t>
   </si>
   <si>
     <t>C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\WAHP</t>
@@ -628,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FCB039-29A7-49D1-BD2D-CAC9DFC1D441}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B14"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -700,7 +691,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>17</v>
@@ -721,8 +712,8 @@
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>39</v>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>22</v>
@@ -744,7 +735,7 @@
         <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>30</v>
@@ -755,7 +746,7 @@
         <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>31</v>
@@ -766,7 +757,7 @@
         <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>42</v>
@@ -814,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:B46"/>
+    <sheetView topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -859,7 +850,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -936,18 +927,18 @@
         <v>28</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>31</v>
@@ -971,7 +962,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -992,7 +983,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>4</v>
@@ -1081,7 +1072,7 @@
         <v>28</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>30</v>
@@ -1092,7 +1083,7 @@
         <v>29</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>31</v>
@@ -1111,7 +1102,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1220,7 +1211,7 @@
         <v>28</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>30</v>
@@ -1231,7 +1222,7 @@
         <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Updated the workflow for uploading renamed files to SharePoint
</commit_message>
<xml_diff>
--- a/WAHPConfigFile.xlsx
+++ b/WAHPConfigFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Desktop\UiPath Projects\WAHPMatchingAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D26233-92AE-4905-BD30-EE85DB539E43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CC1EA7-A13E-47B7-B45C-DC27C3BFB6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -69,9 +69,6 @@
     <t>%2FDONE&amp;viewid=0cafe987%2D9ce0%2D4c52%2Dbaeb%2D28681de003dc</t>
   </si>
   <si>
-    <t>C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Desktop\FLOBOT\</t>
-  </si>
-  <si>
     <t>SharePoint site's FLOBOT folder - base URL</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>ZippedDirectory</t>
   </si>
   <si>
-    <t>C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Desktop\FLOBOT</t>
-  </si>
-  <si>
     <t>Zipped folder directory</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>CC List</t>
   </si>
   <si>
-    <t>E:\Bot_Files\RPA FL Renaming\FLOBOT\</t>
-  </si>
-  <si>
     <t>E:\Bot_Files\RPA FL Renaming\FLOBOT</t>
   </si>
   <si>
@@ -177,9 +168,6 @@
     <t>https://reedelsevier.sharepoint.com/sites/RollanLester/Shared%20Documents/Forms/AllItems.aspx?id=%2Fsites%2FRollanLester%2FShared%20Documents%2FWAHP&amp;viewid=105abaaa%2D085a%2D4a79%2D8458%2D7b6ecbd5487b</t>
   </si>
   <si>
-    <t>C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\WAHP</t>
-  </si>
-  <si>
     <t>WAHP SP to Local Computer - Testing</t>
   </si>
   <si>
@@ -190,6 +178,12 @@
   </si>
   <si>
     <t>doris.cuaresma@lexisnexisrisk.com; shiela.agravante@lexisnexisrisk.com</t>
+  </si>
+  <si>
+    <t>E:\Bot_Files\RPA WAHP Matching Automation\WABOT</t>
+  </si>
+  <si>
+    <t>E:\Bot_Files\RPA WAHP Matching Automation\WABOT\</t>
   </si>
 </sst>
 </file>
@@ -647,7 +641,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -658,10 +652,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -669,10 +663,10 @@
         <v>7</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
@@ -680,87 +674,87 @@
         <v>8</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -805,7 +799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B35" sqref="B35:B41"/>
     </sheetView>
   </sheetViews>
@@ -818,7 +812,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -850,10 +844,10 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -861,10 +855,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -872,87 +866,87 @@
         <v>8</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -962,7 +956,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -983,7 +977,7 @@
         <v>3</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>4</v>
@@ -994,10 +988,10 @@
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -1005,10 +999,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" s="6"/>
     </row>
@@ -1017,92 +1011,92 @@
         <v>8</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1123,7 +1117,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>4</v>
@@ -1134,10 +1128,10 @@
         <v>5</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -1148,7 +1142,7 @@
         <v>9</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -1159,84 +1153,84 @@
         <v>9</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C41" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>